<commit_message>
Modulo instituciones template monster bs4
</commit_message>
<xml_diff>
--- a/assets/formatos_cargue/f34_eliminacion_preguntas_abiertas.xlsx
+++ b/assets/formatos_cargue/f34_eliminacion_preguntas_abiertas.xlsx
@@ -107,7 +107,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">: Elimina solo preguntas abiertas creados por usuarios de instituciones.
+          <t xml:space="preserve">: Elimina solo preguntas abiertas creadas por En Línea Editores.
 </t>
         </r>
         <r>
@@ -127,7 +127,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>: Elimina solo preguntas abiertas creadas por En Línea Editores</t>
+          <t>: Elimina solo preguntas abiertas creadas por usuarios de Instituciones.</t>
         </r>
       </text>
     </comment>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -522,7 +522,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E9:E10"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>